<commit_message>
Fix ID tag in the index.html file
</commit_message>
<xml_diff>
--- a/php/assets/dados.xlsx
+++ b/php/assets/dados.xlsx
@@ -75,7 +75,7 @@
       </c>
       <c r="E1" s="0" t="inlineStr">
         <is>
-          <t>Institution 1</t>
+          <t>Author 1 Institution</t>
         </is>
       </c>
       <c r="F1" s="0" t="inlineStr">
@@ -85,7 +85,7 @@
       </c>
       <c r="G1" s="0" t="inlineStr">
         <is>
-          <t>Institution 2</t>
+          <t>Author 2 Institution</t>
         </is>
       </c>
       <c r="H1" s="0" t="inlineStr">
@@ -95,7 +95,7 @@
       </c>
       <c r="I1" s="0" t="inlineStr">
         <is>
-          <t>Institution 3</t>
+          <t>Author 3 Institution</t>
         </is>
       </c>
       <c r="J1" s="0" t="inlineStr">
@@ -105,7 +105,7 @@
       </c>
       <c r="K1" s="0" t="inlineStr">
         <is>
-          <t>Institution 4</t>
+          <t>Author 4 Institution</t>
         </is>
       </c>
       <c r="L1" s="0" t="inlineStr">
@@ -115,7 +115,7 @@
       </c>
       <c r="M1" s="0" t="inlineStr">
         <is>
-          <t>Institution 5</t>
+          <t>Author 5 Institution</t>
         </is>
       </c>
       <c r="N1" s="0" t="inlineStr">
@@ -125,7 +125,7 @@
       </c>
       <c r="O1" s="0" t="inlineStr">
         <is>
-          <t>Institution 6</t>
+          <t>Author 6 Institution</t>
         </is>
       </c>
       <c r="P1" s="0" t="inlineStr">
@@ -135,7 +135,7 @@
       </c>
       <c r="Q1" s="0" t="inlineStr">
         <is>
-          <t>Institution 7</t>
+          <t>Author 7 Institution</t>
         </is>
       </c>
       <c r="R1" s="0" t="inlineStr">
@@ -145,7 +145,7 @@
       </c>
       <c r="S1" s="0" t="inlineStr">
         <is>
-          <t>Institution 8</t>
+          <t>Author 8 Institution</t>
         </is>
       </c>
       <c r="T1" s="0" t="inlineStr">
@@ -155,13 +155,15 @@
       </c>
       <c r="U1" s="0" t="inlineStr">
         <is>
-          <t>Institution 9</t>
+          <t>Author 9 Institution</t>
         </is>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="0">
-        <v>0</v>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>137458</t>
+        </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
@@ -215,8 +217,10 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="0">
-        <v>0</v>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>137459</t>
+        </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
@@ -240,8 +244,10 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="0">
-        <v>0</v>
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>137460</t>
+        </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
@@ -285,8 +291,10 @@
       </c>
     </row>
     <row r="5" spans="1:35">
-      <c r="A5" s="0">
-        <v>0</v>
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>137464</t>
+        </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
@@ -460,8 +468,10 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="0">
-        <v>0</v>
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>137465</t>
+        </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -525,8 +535,10 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="0">
-        <v>0</v>
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>137466</t>
+        </is>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
@@ -570,8 +582,10 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="0">
-        <v>0</v>
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>137468</t>
+        </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
@@ -605,8 +619,10 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="0">
-        <v>0</v>
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>137469</t>
+        </is>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
@@ -680,8 +696,10 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="0">
-        <v>0</v>
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>137470</t>
+        </is>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
@@ -725,8 +743,10 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="0">
-        <v>0</v>
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>137471</t>
+        </is>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
@@ -790,8 +810,10 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="0">
-        <v>0</v>
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>137472</t>
+        </is>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
@@ -845,8 +867,10 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="0">
-        <v>0</v>
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>137473</t>
+        </is>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
@@ -890,8 +914,10 @@
       </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="0">
-        <v>0</v>
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>137474</t>
+        </is>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
@@ -995,8 +1021,10 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="0">
-        <v>0</v>
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>137476</t>
+        </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
@@ -1090,8 +1118,10 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="0">
-        <v>0</v>
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>137477</t>
+        </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
@@ -1125,8 +1155,10 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="0">
-        <v>0</v>
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>137478</t>
+        </is>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
@@ -1170,8 +1202,10 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="0">
-        <v>0</v>
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>137479</t>
+        </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
@@ -1245,8 +1279,10 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="0">
-        <v>0</v>
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>137480</t>
+        </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
@@ -1280,8 +1316,10 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="0">
-        <v>0</v>
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>137486</t>
+        </is>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
@@ -1335,8 +1373,10 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="0">
-        <v>0</v>
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>137487</t>
+        </is>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
@@ -1390,8 +1430,10 @@
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="0">
-        <v>0</v>
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>137555</t>
+        </is>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
@@ -1455,8 +1497,10 @@
       </c>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="0">
-        <v>0</v>
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>137556</t>
+        </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
@@ -1540,8 +1584,10 @@
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="0">
-        <v>0</v>
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>139165</t>
+        </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
@@ -1595,8 +1641,10 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="0">
-        <v>0</v>
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>139166</t>
+        </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
@@ -1620,8 +1668,10 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="0">
-        <v>0</v>
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>139167</t>
+        </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
@@ -1645,8 +1695,10 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="0">
-        <v>0</v>
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>139168</t>
+        </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
@@ -1670,8 +1722,10 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="0">
-        <v>0</v>
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>139169</t>
+        </is>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
@@ -1695,8 +1749,10 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="0">
-        <v>0</v>
+      <c r="A29" s="0" t="inlineStr">
+        <is>
+          <t>139170</t>
+        </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
@@ -1730,8 +1786,10 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="0">
-        <v>0</v>
+      <c r="A30" s="0" t="inlineStr">
+        <is>
+          <t>139172</t>
+        </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
@@ -1755,8 +1813,10 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="0">
-        <v>0</v>
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>139173</t>
+        </is>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
@@ -1780,8 +1840,10 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="0">
-        <v>0</v>
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>139174</t>
+        </is>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
@@ -1805,8 +1867,10 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="0">
-        <v>0</v>
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>139175</t>
+        </is>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
@@ -1830,8 +1894,10 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="0">
-        <v>0</v>
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>139176</t>
+        </is>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
@@ -1855,8 +1921,10 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="0">
-        <v>0</v>
+      <c r="A35" s="0" t="inlineStr">
+        <is>
+          <t>139177</t>
+        </is>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
@@ -1880,8 +1948,10 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="0">
-        <v>0</v>
+      <c r="A36" s="0" t="inlineStr">
+        <is>
+          <t>139178</t>
+        </is>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
@@ -1905,8 +1975,10 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="0">
-        <v>0</v>
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>139180</t>
+        </is>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
@@ -1930,8 +2002,10 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="0">
-        <v>0</v>
+      <c r="A38" s="0" t="inlineStr">
+        <is>
+          <t>139181</t>
+        </is>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
@@ -1975,8 +2049,10 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="0">
-        <v>0</v>
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>139183</t>
+        </is>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
@@ -2000,8 +2076,10 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="0">
-        <v>0</v>
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>139184</t>
+        </is>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
@@ -2025,8 +2103,10 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="0">
-        <v>0</v>
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>139185</t>
+        </is>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
@@ -2060,8 +2140,10 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="0">
-        <v>0</v>
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>139186</t>
+        </is>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
@@ -2085,8 +2167,10 @@
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="0">
-        <v>0</v>
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t>139187</t>
+        </is>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
@@ -2110,8 +2194,10 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="0">
-        <v>0</v>
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>139188</t>
+        </is>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
@@ -2135,8 +2221,10 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="0">
-        <v>0</v>
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>139190</t>
+        </is>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
@@ -2160,8 +2248,10 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="0">
-        <v>0</v>
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>139192</t>
+        </is>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
@@ -2185,8 +2275,10 @@
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="0">
-        <v>0</v>
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t>139193</t>
+        </is>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
@@ -2210,8 +2302,10 @@
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="0">
-        <v>0</v>
+      <c r="A48" s="0" t="inlineStr">
+        <is>
+          <t>139194</t>
+        </is>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
@@ -2255,8 +2349,10 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="0">
-        <v>0</v>
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t>139195</t>
+        </is>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
@@ -2280,8 +2376,10 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="0">
-        <v>0</v>
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t>139189</t>
+        </is>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
@@ -2305,8 +2403,10 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="0">
-        <v>0</v>
+      <c r="A51" s="0" t="inlineStr">
+        <is>
+          <t>139191</t>
+        </is>
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
@@ -2330,8 +2430,10 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="0">
-        <v>0</v>
+      <c r="A52" s="0" t="inlineStr">
+        <is>
+          <t>139179</t>
+        </is>
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
@@ -2355,8 +2457,10 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="0">
-        <v>0</v>
+      <c r="A53" s="0" t="inlineStr">
+        <is>
+          <t>139171</t>
+        </is>
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
@@ -2380,8 +2484,10 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="0">
-        <v>0</v>
+      <c r="A54" s="0" t="inlineStr">
+        <is>
+          <t>137467</t>
+        </is>
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
@@ -2445,8 +2551,10 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="0">
-        <v>0</v>
+      <c r="A55" s="0" t="inlineStr">
+        <is>
+          <t>139182</t>
+        </is>
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
@@ -2470,8 +2578,10 @@
       </c>
     </row>
     <row r="56" spans="1:39">
-      <c r="A56" s="0">
-        <v>0</v>
+      <c r="A56" s="0" t="inlineStr">
+        <is>
+          <t>137461</t>
+        </is>
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
@@ -2665,8 +2775,10 @@
       </c>
     </row>
     <row r="57" spans="1:29">
-      <c r="A57" s="0">
-        <v>0</v>
+      <c r="A57" s="0" t="inlineStr">
+        <is>
+          <t>137462</t>
+        </is>
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
@@ -2810,8 +2922,10 @@
       </c>
     </row>
     <row r="58" spans="1:17">
-      <c r="A58" s="0">
-        <v>0</v>
+      <c r="A58" s="0" t="inlineStr">
+        <is>
+          <t>137475</t>
+        </is>
       </c>
       <c r="B58" s="0" t="inlineStr">
         <is>
@@ -2890,8 +3004,10 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="0">
-        <v>0</v>
+      <c r="A59" s="0" t="inlineStr">
+        <is>
+          <t>139532</t>
+        </is>
       </c>
       <c r="B59" s="0" t="inlineStr">
         <is>
@@ -2915,8 +3031,10 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="0">
-        <v>0</v>
+      <c r="A60" s="0" t="inlineStr">
+        <is>
+          <t>139533</t>
+        </is>
       </c>
       <c r="B60" s="0" t="inlineStr">
         <is>
@@ -2940,8 +3058,10 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="0">
-        <v>0</v>
+      <c r="A61" s="0" t="inlineStr">
+        <is>
+          <t>139534</t>
+        </is>
       </c>
       <c r="B61" s="0" t="inlineStr">
         <is>
@@ -2965,8 +3085,10 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="0">
-        <v>0</v>
+      <c r="A62" s="0" t="inlineStr">
+        <is>
+          <t>139531</t>
+        </is>
       </c>
       <c r="B62" s="0" t="inlineStr">
         <is>
@@ -2990,8 +3112,10 @@
       </c>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="0">
-        <v>0</v>
+      <c r="A63" s="0" t="inlineStr">
+        <is>
+          <t>137463</t>
+        </is>
       </c>
       <c r="B63" s="0" t="inlineStr">
         <is>

</xml_diff>